<commit_message>
new rules & cards
</commit_message>
<xml_diff>
--- a/Cards/List of card effects.xlsx
+++ b/Cards/List of card effects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viikt\OneDrive\Documents\My Games\Tabletop Simulator\Mods\Ghost board game\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealProjects\Ghost-Board-Game\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D15B51F-15AD-4D53-A49B-8828E658EF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFFC640-5479-4799-9FF8-1395F9459DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41385" yWindow="1590" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Bomb: Destroy a tile and its adjecent ones (+ shape)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Steal one limb from an opponent</t>
   </si>
@@ -36,28 +33,46 @@
     <t xml:space="preserve"> +2 movement for the next round</t>
   </si>
   <si>
-    <t>Send an opponent back to the gravekeeper</t>
-  </si>
-  <si>
-    <t>Floatie: Float past a water tile (one time use)</t>
-  </si>
-  <si>
-    <t>Ice pick: Hack through an icy path</t>
-  </si>
-  <si>
     <t>Redraw: Return any amount of tiles to the bag and draw new ones</t>
   </si>
   <si>
-    <t>Ambush: Challenge another player to rock, paper, scissors. If you win, take one of their limbs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sabotage: nullify another player's card action. </t>
   </si>
   <si>
     <t>Switch places with another player.</t>
   </si>
   <si>
-    <t>Pick up any tile and place it down anywhere. (including your hand if you have less than 5)</t>
+    <t xml:space="preserve">Bomb: Destroy a tile and its adjecent ones (+ shape).  Tiles go back to pile. Can't destroy tile under player.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All the ground tiles get removed except the ones players stand on. </t>
+  </si>
+  <si>
+    <t>Send an opponent back to the cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move vendor to the spot nearest to you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up any tile from the map and place it down anywhere. </t>
+  </si>
+  <si>
+    <t>Choose 1 player that wont be able to place any tiles for the next round.</t>
+  </si>
+  <si>
+    <t>All bonuses from the leg limbs  are disabled for this turn</t>
+  </si>
+  <si>
+    <t>All bonuses from the arm limbs  are disabled for this turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push other player in any direction up to 4 steps. (cant place them on tiles they cant pass). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destroy a raw of tiles up to 4. </t>
+  </si>
+  <si>
+    <t>Slide an entire raw of tiles and players that stand on it in any direction.  Tiles over dog spots/ outside map get destroyed</t>
   </si>
 </sst>
 </file>
@@ -375,70 +390,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="198" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="79.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="8" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rules need new pdf
</commit_message>
<xml_diff>
--- a/Cards/List of card effects.xlsx
+++ b/Cards/List of card effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealProjects\Ghost-Board-Game\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D62B48-C65E-48FC-9883-B667D6ACE5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57D7C28-7DA7-4F21-B833-2FA43F742009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,15 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Redraw: Return any amount of tiles to the bag and draw new ones</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sabotage: nullify another player's card action. </t>
   </si>
   <si>
-    <t xml:space="preserve">Bomb: Destroy a tile and its adjecent ones (+ shape).  Tiles go back to pile. Can't destroy tile under player.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fair Trade: Move vendor (dog) to the spot nearest to you </t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>Slide: Slide an entire raw of tiles and players that stand on it in any direction.  Tiles over dog spots/ outside map get destroyed</t>
+  </si>
+  <si>
+    <t>Redraw: Return any amount of tiles to the bag and draw new ones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bomb: Destroy a tile and its adjacent ones (+ shape).  Tiles go back to pile. Can't destroy tile under player.  </t>
   </si>
 </sst>
 </file>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="198" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="198" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -403,82 +403,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>